<commit_message>
resloving the closing browser issue
</commit_message>
<xml_diff>
--- a/PythonPrograms/sample.xlsx
+++ b/PythonPrograms/sample.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="map.contact_board" sheetId="1" r:id="rId1"/>
+    <sheet name="map.contact_education" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Req</t>
   </si>
@@ -55,76 +55,40 @@
     <t>1</t>
   </si>
   <si>
-    <t>TC01_Onbaording the map.contact_board   into MDM Raw layer.</t>
-  </si>
-  <si>
-    <t>TC00_Countvalidation_map.contact_board</t>
+    <t>TC01_Onbaording the map.contact_education   into MDM Raw layer.</t>
+  </si>
+  <si>
+    <t>TC00_Countvalidation_map.contact_education</t>
   </si>
   <si>
     <t>TC_Verification of duplicates in the data</t>
   </si>
   <si>
-    <t>TC_TransformationCheck_startdate</t>
-  </si>
-  <si>
-    <t>TC_TransformationCheck_enddate</t>
-  </si>
-  <si>
-    <t>TC_TransformationCheck_AccountID</t>
-  </si>
-  <si>
-    <t>TC_TransformationCheck_AccountName</t>
-  </si>
-  <si>
-    <t>TC_TransformationCheck_BoardSpecificCommittee</t>
-  </si>
-  <si>
-    <t>TC_TransformationCheck_ BoardRole</t>
-  </si>
-  <si>
-    <t>TC_TransformationCheck_BoardMemberFlag</t>
-  </si>
-  <si>
-    <t>TC_Verification of structure for onbaordingmap.contact_board</t>
+    <t>TC_TransformationCheck_Extract the data from the table in the MDM Map Layer using  below query</t>
+  </si>
+  <si>
+    <t>TC_Verification of structure for onbaordingmap.contact_education</t>
   </si>
   <si>
     <t>TC_Verification of count between the source and target table</t>
   </si>
   <si>
-    <t>Check whether there  any duplicates exists on the latest processID in map.contact_boardtable.</t>
-  </si>
-  <si>
-    <t>TC_Verify whether the transformation logic has applied as per the requirement document for the column  startdate</t>
-  </si>
-  <si>
-    <t>TC_Verify whether the transformation logic has applied as per the requirement document for the column  enddate</t>
-  </si>
-  <si>
-    <t>TC_Verify whether the transformation logic has applied as per the requirement document for the column  AccountID</t>
-  </si>
-  <si>
-    <t>TC_Verify whether the transformation logic has applied as per the requirement document for the column  AccountName</t>
-  </si>
-  <si>
-    <t>TC_Verify whether the transformation logic has applied as per the requirement document for the column  BoardSpecificCommittee</t>
-  </si>
-  <si>
-    <t>TC_Verify whether the transformation logic has applied as per the requirement document for the column   BoardRole</t>
-  </si>
-  <si>
-    <t>TC_Verify whether the transformation logic has applied as per the requirement document for the column  BoardMemberFlag</t>
+    <t>Check whether there  any duplicates exists on the latest processID in map.contact_educationtable.</t>
+  </si>
+  <si>
+    <t>TC_Verify whether the transformation logic has applied as per the requirement document for the column  Extract the data from the table in the MDM Map Layer using  below query</t>
   </si>
   <si>
     <t xml:space="preserve"> Open the Microsoft SQL Server,Go to the Databases folder and expand it. 
-                Go to the Tables folder right click on the map.contact_boardtable a new window will open with metadata. 
-                Go to the Tables folder right click on the map.contact_boardtable a new window will open with metadata. 
+                Go to the Tables folder right click on the map.contact_educationtable a new window will open with metadata. 
+                Go to the Tables folder right click on the map.contact_educationtable a new window will open with metadata. 
                 Verify the struture of the both the tables. </t>
   </si>
   <si>
     <t xml:space="preserve"> Verify the count of the source table using below query in the MDM Raw Layer 
  select count(*) from crm.s_contact where change_flag= 'Y' 
                    Verify the count of the target table using below query in the MDM MAP layer 
- select count(*) from map.contact_board 
+ select count(*) from map.contact_education 
                    Note: Please apply processID filter for both the tables Verify the count between the  source and target table. </t>
   </si>
   <si>
@@ -132,92 +96,27 @@
   </si>
   <si>
     <t>Extract the data from the table in the MDM Raw Layer using  below query
-SELECT  c1.row_id, p1.START_DT 
-FROM CRM.S_ORG_EXT o1 LEFT OUTER JOIN CRM.S_PARTY_PER p1
-ON o1.ROW_ID = p1.PARTY_ID LEFT OUTER JOIN CRM.S_CONTACT c1 ON p1.PERSON_ID=c1.ROW_ID 
- WHERE o1.PROCESSID='$latestProcessId' AND p1.CHANGE_FLAG='Y' and c1.change_flag = 'Y'
- and o1.change_flag = 'Y' and p1.processid = '$LatestProcessID'
-and c1.ROW_ID IN (SELECT ROW_ID FROM CRM.CONTACTID_STG WHERE PROCESSID='$LatestProcessID') 
-and p1.PARTY_ID IS NOT NULL and p1.X_CONTACT_CLASS = 'Board' Extract the data from the table in the MDM Map Layer using  below query 
- select mdmid,  startdate map.contact_board 
- Data Validation:  Verify the data from Source Query and Target Query  i.e by applying the except query.   
-Note: Please apply processID filter while validating the data for both the above mentioned tables.</t>
+SourceQuery: 'select row_id,'Degree' as EducationTypeCode from crm.s_Contact where 1=1 and c1.ROW_ID IN (SELECT ROW_ID FROM CRM.CONTACTID_STG WHERE PROCESSID='$LatestProcessID')  and change_flag = 'Y' Extract the data from the table in the MDM Map Layer using  below query 
+ TargetQuery: select row_id,EducationTypeCode   from map.contact_education Data Validation:  Verify the data from Source Query and Target Query  i.e by applying the except query.   
+ Note: Please apply processID filter while validating the data for both the above mentioned tables.</t>
   </si>
   <si>
     <t>Extract the data from the table in the MDM Raw Layer using  below query
-SELECT  c1.row_id, p1.end_Dt 
-FROM CRM.S_ORG_EXT o1 LEFT OUTER JOIN CRM.S_PARTY_PER p1
-ON o1.ROW_ID = p1.PARTY_ID LEFT OUTER JOIN CRM.S_CONTACT c1 ON p1.PERSON_ID=c1.ROW_ID 
- WHERE o1.PROCESSID='$latestProcessId' AND p1.CHANGE_FLAG='Y' and c1.change_flag = 'Y'
- and o1.change_flag = 'Y' and p1.processid = '$LatestProcessID'
-and c1.ROW_ID IN (SELECT ROW_ID FROM CRM.CONTACTID_STG WHERE PROCESSID='$LatestProcessID') 
-and p1.PARTY_ID IS NOT NULL and p1.X_CONTACT_CLASS = 'Board' Extract the data from the table in the MDM Map Layer using  below query 
- select mdmid,  enddate map.contact_board 
- Data Validation:  Verify the data from Source Query and Target Query  i.e by applying the except query.   
-Note: Please apply processID filter while validating the data for both the above mentioned tables.</t>
+SourceQuery: select row_id, CASE WHEN c1.DEGREE IS NULL THEN 'Not Provided' ELSE SRC1.DEGREE END EducationDegree from crm.s_Contact where 1=1 and c1.ROW_ID IN (SELECT ROW_ID FROM CRM.CONTACTID_STG WHERE PROCESSID='$LatestProcessID')  and change_flag = 'Y' Extract the data from the table in the MDM Map Layer using  below query 
+ TargetQuery: select row_id,EducationDegree  from map.contact_education Data Validation:  Verify the data from Source Query and Target Query  i.e by applying the except query.   
+ Note: Please apply processID filter while validating the data for both the above mentioned tables.</t>
   </si>
   <si>
     <t>Extract the data from the table in the MDM Raw Layer using  below query
-SELECT  c1.row_id,CASE WHEN  p1.PARTY_ID IS NULL THEN 'Not Provided' ELSE  p1.PARTY_ID END AccountID
-FROM CRM.S_ORG_EXT o1 LEFT OUTER JOIN CRM.S_PARTY_PER p1
-ON o1.ROW_ID = p1.PARTY_ID LEFT OUTER JOIN CRM.S_CONTACT c1 ON p1.PERSON_ID=c1.ROW_ID 
- WHERE o1.PROCESSID='$latestProcessId' AND p1.CHANGE_FLAG='Y' and c1.change_flag = 'Y'
- and o1.change_flag = 'Y' and p1.processid = '$LatestProcessID'
-and c1.ROW_ID IN (SELECT ROW_ID FROM CRM.CONTACTID_STG WHERE PROCESSID='$LatestProcessID') 
-and p1.PARTY_ID IS NOT NULL and p1.X_CONTACT_CLASS = 'Board' Extract the data from the table in the MDM Map Layer using  below query 
- select mdmid,  AccountID map.contact_board 
- Data Validation:  Verify the data from Source Query and Target Query  i.e by applying the except query.   
-Note: Please apply processID filter while validating the data for both the above mentioned tables.</t>
+SourceQuery: select row_id, c2.ATTRIB_04 as EducationBackground  from crm.s_Contact c1, crm.s_contact_x c2 where 1=1 and c1.row_id = c2.row_id  and c1.ROW_ID IN (SELECT ROW_ID FROM CRM.CONTACTID_STG WHERE PROCESSID='$LatestProcessID')  and change_flag = 'Y' Extract the data from the table in the MDM Map Layer using  below query 
+ TargetQuery: select row_id,EducationBackground   from map.contact_education Data Validation:  Verify the data from Source Query and Target Query  i.e by applying the except query.   
+ Note: Please apply processID filter while validating the data for both the above mentioned tables.</t>
   </si>
   <si>
     <t>Extract the data from the table in the MDM Raw Layer using  below query
-SELECT  c1.row_id,CASE WHEN o1.NAME IS NULL THEN 'Not Provided' ELSE o1.NAME END AccountIName
-FROM CRM.S_ORG_EXT o1 LEFT OUTER JOIN CRM.S_PARTY_PER p1
-ON o1.ROW_ID = p1.PARTY_ID LEFT OUTER JOIN CRM.S_CONTACT c1 ON p1.PERSON_ID=c1.ROW_ID 
- WHERE o1.PROCESSID='$latestProcessId'  AND p1.CHANGE_FLAG='Y' and c1.change_flag = 'Y'
- and o1.change_flag = 'Y' and p1.processid = '$LatestProcessID'
-and c1.ROW_ID IN (SELECT ROW_ID FROM CRM.CONTACTID_STG WHERE PROCESSID='$LatestProcessID') 
-and  o1.NAME IS NOT NULL and p1.X_CONTACT_CLASS = 'Board' Extract the data from the table in the MDM Map Layer using  below query 
- select mdmid,  AccountName map.contact_board 
- Data Validation:  Verify the data from Source Query and Target Query  i.e by applying the except query.   
-Note: Please apply processID filter while validating the data for both the above mentioned tables.</t>
-  </si>
-  <si>
-    <t>Extract the data from the table in the MDM Raw Layer using  below query
-SELECT c1.row_id, CASE WHEN p1.X_JOB_DEPT IS NULL THEN 'Not Provided' ELSE p1.X_JOB_DEPT END BoardSpecificCommittee
-FROM CRM.S_ORG_EXT o1 LEFT OUTER JOIN CRM.S_PARTY_PER p1
-ON o1.ROW_ID = p1.PARTY_ID LEFT OUTER JOIN CRM.S_CONTACT c1 ON p1.PERSON_ID=c1.ROW_ID 
- WHERE o1.PROCESSID='$latestProcessId' AND p1.CHANGE_FLAG='Y' and c1.change_flag = 'Y'
- and o1.change_flag = 'Y' and p1.processid = '$LatestProcessID'
-and c1.ROW_ID IN (SELECT ROW_ID FROM CRM.CONTACTID_STG WHERE PROCESSID='$LatestProcessID') 
-and p1.X_JOB_DEPT IS NOT NULL and p1.X_CONTACT_CLASS = 'Board' Extract the data from the table in the MDM Map Layer using  below query 
- select mdmid,  BoardSpecificCommittee map.contact_board 
- Data Validation:  Verify the data from Source Query and Target Query  i.e by applying the except query.   
-Note: Please apply processID filter while validating the data for both the above mentioned tables.</t>
-  </si>
-  <si>
-    <t>Extract the data from the table in the MDM Raw Layer using  below query
-SELECT c1.row_id,p1.X_JOB_TITLE_LEVEL AS BoardRole FROM CRM.S_ORG_EXT o1 LEFT OUTER JOIN CRM.S_PARTY_PER p1
-ON o1.ROW_ID = p1.PARTY_ID LEFT OUTER JOIN CRM.S_CONTACT c1 ON p1.PERSON_ID=c1.ROW_ID 
- WHERE o1.PROCESSID='$latestProcessId'  AND p1.CHANGE_FLAG='Y' and c1.change_flag = 'Y'
- and o1.change_flag = 'Y' and p1.processid = '$LatestProcessID'
-and c1.ROW_ID IN (SELECT ROW_ID FROM CRM.CONTACTID_STG WHERE PROCESSID='$LatestProcessID') 
-and p1.X_JOB_TITLE_LEVEL IS NOT NULL and p1.X_CONTACT_CLASS = 'Board' Extract the data from the table in the MDM Map Layer using  below query 
- select mdmid,   BoardRole map.contact_board 
- Data Validation:  Verify the data from Source Query and Target Query  i.e by applying the except query.   
-Note: Please apply processID filter while validating the data for both the above mentioned tables.</t>
-  </si>
-  <si>
-    <t>Extract the data from the table in the MDM Raw Layer using  below query
-SELECT c1.row_id,SUBSTRING(B.BOARD_SEAT_FLG,1,10)  FROM CRM.S_ORG_EXT o1 LEFT OUTER JOIN CRM.S_PARTY_PER p1
-ON o1.ROW_ID = p1.PARTY_ID LEFT OUTER JOIN CRM.S_CONTACT c1 ON p1.PERSON_ID=c1.ROW_ID 
- WHERE o1.PROCESSID='$latestProcessId'  AND p1.CHANGE_FLAG='Y' and c1.change_flag = 'Y'
- and o1.change_flag = 'Y' and p1.processid = '$LatestProcessID'
-and c1.ROW_ID IN (SELECT ROW_ID FROM CRM.CONTACTID_STG WHERE PROCESSID='$LatestProcessID') 
-and p1.BoardMemberFlag IS NOT NULL and p1.X_CONTACT_CLASS = 'Board' Extract the data from the table in the MDM Map Layer using  below query 
- select mdmid,  BoardMemberFlag map.contact_board 
- Data Validation:  Verify the data from Source Query and Target Query  i.e by applying the except query.   
-Note: Please apply processID filter while validing the data for both the above mentioned tables.</t>
+SourceQuery: select row_id, c2.X_ALUM_HON_QUAL AS Qualifications  from crm.s_Contact c1, crm.s_contact_x c2 where 1=1 and c1.row_id = c2.row_id  and c1.ROW_ID IN (SELECT ROW_ID FROM CRM.CONTACTID_STG WHERE PROCESSID='$LatestProcessID')  and change_flag = 'Y' Extract the data from the table in the MDM Map Layer using  below query 
+ TargetQuery: select row_id,Qualifications    from map.contact_education Data Validation:  Verify the data from Source Query and Target Query  i.e by applying the except query.   
+ Note: Please apply processID filter while validating the data for both the above mentioned tables.</t>
   </si>
   <si>
     <t>Structure should match between Source and Target table.</t>
@@ -227,7 +126,7 @@
   </si>
   <si>
     <t xml:space="preserve">Below Query will be used to identify the duplicates  
-                select mdmid,count(*) from map.contact_boardwhere 1=1 group by mdmid having count(*) 
+                select mdmid,count(*) from map.contact_educationwhere 1=1 group by mdmid having count(*) 
                 Note: Please apply processID filter while validating the data  </t>
   </si>
   <si>
@@ -237,25 +136,7 @@
     <t xml:space="preserve"> Duplicates should not exists on the latest processID. We should have all unique records </t>
   </si>
   <si>
-    <t>startdate  value should match between the Source and Target tables</t>
-  </si>
-  <si>
-    <t>enddate  value should match between the Source and Target tables</t>
-  </si>
-  <si>
-    <t>AccountID  value should match between the Source and Target tables</t>
-  </si>
-  <si>
-    <t>AccountName  value should match between the Source and Target tables</t>
-  </si>
-  <si>
-    <t>BoardSpecificCommittee  value should match between the Source and Target tables</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BoardRole  value should match between the Source and Target tables</t>
-  </si>
-  <si>
-    <t>BoardMemberFlag  value should match between the Source and Target tables</t>
+    <t>Extract the data from the table in the MDM Map Layer using  below query  value should match between the Source and Target tables</t>
   </si>
 </sst>
 </file>
@@ -616,7 +497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -681,19 +562,19 @@
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -707,19 +588,19 @@
         <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -733,19 +614,19 @@
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -756,19 +637,19 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -776,22 +657,22 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -799,22 +680,22 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -822,91 +703,22 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="2">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="2">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="2">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>